<commit_message>
update for single zero
</commit_message>
<xml_diff>
--- a/textXlTrail.xlsx
+++ b/textXlTrail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maksymv/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FCD0FA0-24F0-ED4D-B20F-5A3BA9542F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0CCA5D-D8A4-3345-9550-8010713D6770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{000E7108-3E9B-1E44-AB8C-CDD0D2392ED3}"/>
   </bookViews>
@@ -464,7 +464,7 @@
   <dimension ref="A3:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,18 +491,18 @@
         <v>5</v>
       </c>
       <c r="B4" s="4">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4">
-        <f>C4/38</f>
-        <v>2.6315789473684209E-2</v>
+        <f>C4/37</f>
+        <v>2.7027027027027029E-2</v>
       </c>
       <c r="E4" s="5">
         <f>B4*D4</f>
-        <v>0.94736842105263153</v>
+        <v>1.0270270270270272</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -516,12 +516,12 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D11" si="0">C5/38</f>
-        <v>5.2631578947368418E-2</v>
+        <f t="shared" ref="D5:D11" si="0">C5/37</f>
+        <v>5.4054054054054057E-2</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" ref="E5:E11" si="1">B5*D5</f>
-        <v>0.94736842105263153</v>
+        <v>0.97297297297297303</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -536,11 +536,11 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>7.8947368421052627E-2</v>
+        <v>8.1081081081081086E-2</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="1"/>
-        <v>0.94736842105263153</v>
+        <v>0.97297297297297303</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -555,11 +555,11 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.10526315789473684</v>
+        <v>0.10810810810810811</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="1"/>
-        <v>0.94736842105263153</v>
+        <v>0.97297297297297303</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -574,11 +574,11 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0.15789473684210525</v>
+        <v>0.16216216216216217</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="1"/>
-        <v>0.94736842105263153</v>
+        <v>0.97297297297297303</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -586,18 +586,18 @@
         <v>10</v>
       </c>
       <c r="B9" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="4">
         <v>12</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.31578947368421051</v>
+        <v>0.32432432432432434</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="1"/>
-        <v>0.94736842105263153</v>
+        <v>1.2972972972972974</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -612,11 +612,11 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0.47368421052631576</v>
+        <v>0.48648648648648651</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" si="1"/>
-        <v>0.94736842105263153</v>
+        <v>0.97297297297297303</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -631,11 +631,11 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>0.13157894736842105</v>
+        <v>0.13513513513513514</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="1"/>
-        <v>0.92105263157894735</v>
+        <v>0.94594594594594605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>